<commit_message>
xong excel, bieu do
</commit_message>
<xml_diff>
--- a/admin/template.xlsx
+++ b/admin/template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\doan_xuan17_thanh_toan\admin\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFC8E959-1EAD-4A37-A7D2-3BB1228C3B0D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18470913-891E-462E-A70D-8BDDFF342066}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" xr2:uid="{C7D51470-7B38-4D27-B357-DAE926002F30}"/>
   </bookViews>
@@ -173,14 +173,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -188,34 +182,34 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -613,8 +607,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59F35B44-676D-4F23-A847-B3E70FD7B37A}">
   <dimension ref="A1:F19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19:F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -627,163 +621,169 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="33" customHeight="1">
-      <c r="A1" s="12"/>
-      <c r="B1" s="12"/>
-      <c r="C1" s="6" t="s">
+      <c r="A1" s="13"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
     </row>
     <row r="2" spans="1:6">
-      <c r="A2" s="12"/>
-      <c r="B2" s="12"/>
-      <c r="C2" s="7" t="s">
+      <c r="A2" s="13"/>
+      <c r="B2" s="13"/>
+      <c r="C2" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="10"/>
     </row>
     <row r="3" spans="1:6" ht="33" customHeight="1">
-      <c r="A3" s="12"/>
-      <c r="B3" s="12"/>
-      <c r="C3" s="7"/>
-      <c r="D3" s="7"/>
-      <c r="E3" s="7"/>
-      <c r="F3" s="7"/>
+      <c r="A3" s="13"/>
+      <c r="B3" s="13"/>
+      <c r="C3" s="10"/>
+      <c r="D3" s="10"/>
+      <c r="E3" s="10"/>
+      <c r="F3" s="10"/>
     </row>
     <row r="4" spans="1:6" ht="18.600000000000001" customHeight="1">
-      <c r="A4" s="12"/>
-      <c r="B4" s="12"/>
-      <c r="C4" s="8" t="s">
+      <c r="A4" s="13"/>
+      <c r="B4" s="13"/>
+      <c r="C4" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="8"/>
-      <c r="E4" s="8"/>
-      <c r="F4" s="8"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
     </row>
     <row r="5" spans="1:6">
-      <c r="A5" s="12"/>
-      <c r="B5" s="12"/>
+      <c r="A5" s="13"/>
+      <c r="B5" s="13"/>
     </row>
     <row r="8" spans="1:6" ht="20.399999999999999" customHeight="1">
-      <c r="A8" s="9" t="s">
+      <c r="A8" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="10"/>
-      <c r="C8" s="10"/>
-      <c r="D8" s="10"/>
-      <c r="E8" s="10"/>
-      <c r="F8" s="10"/>
+      <c r="B8" s="12"/>
+      <c r="C8" s="12"/>
+      <c r="D8" s="12"/>
+      <c r="E8" s="12"/>
+      <c r="F8" s="12"/>
     </row>
     <row r="9" spans="1:6" ht="23.4" customHeight="1">
-      <c r="A9" s="10"/>
-      <c r="B9" s="10"/>
-      <c r="C9" s="10"/>
-      <c r="D9" s="10"/>
-      <c r="E9" s="10"/>
-      <c r="F9" s="10"/>
+      <c r="A9" s="12"/>
+      <c r="B9" s="12"/>
+      <c r="C9" s="12"/>
+      <c r="D9" s="12"/>
+      <c r="E9" s="12"/>
+      <c r="F9" s="12"/>
     </row>
     <row r="10" spans="1:6">
-      <c r="A10" s="11" t="s">
+      <c r="A10" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="11"/>
-      <c r="C10" s="11" t="s">
+      <c r="B10" s="6"/>
+      <c r="C10" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="D10" s="11" t="s">
+      <c r="D10" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="E10" s="11"/>
-      <c r="F10" s="11"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
     </row>
     <row r="11" spans="1:6">
-      <c r="A11" s="11"/>
-      <c r="B11" s="11"/>
-      <c r="C11" s="11"/>
-      <c r="D11" s="11"/>
-      <c r="E11" s="11"/>
-      <c r="F11" s="11"/>
+      <c r="A11" s="6"/>
+      <c r="B11" s="6"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="6"/>
     </row>
     <row r="12" spans="1:6" ht="15">
-      <c r="A12" s="15"/>
-      <c r="B12" s="15"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="14"/>
-      <c r="E12" s="14"/>
-      <c r="F12" s="14"/>
+      <c r="A12" s="8"/>
+      <c r="B12" s="8"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="7"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="7"/>
     </row>
     <row r="13" spans="1:6" ht="15">
-      <c r="A13" s="4"/>
-      <c r="B13" s="4"/>
-      <c r="C13" s="3"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="5"/>
-      <c r="F13" s="5"/>
+      <c r="A13" s="2"/>
+      <c r="B13" s="2"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
     </row>
     <row r="14" spans="1:6" ht="15">
-      <c r="A14" s="4"/>
-      <c r="B14" s="4"/>
-      <c r="C14" s="3"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="5"/>
-      <c r="F14" s="5"/>
+      <c r="A14" s="2"/>
+      <c r="B14" s="2"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
     </row>
     <row r="15" spans="1:6" ht="15">
-      <c r="A15" s="3"/>
-      <c r="B15" s="3"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
+      <c r="A15" s="1"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
     </row>
     <row r="16" spans="1:6" ht="15.6">
-      <c r="A16" s="3"/>
-      <c r="B16" s="3"/>
-      <c r="C16" s="3"/>
-      <c r="D16" s="13" t="s">
+      <c r="A16" s="1"/>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E16" s="13"/>
-      <c r="F16" s="13"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="4"/>
     </row>
     <row r="17" spans="1:6" ht="15">
-      <c r="A17" s="3"/>
-      <c r="B17" s="3"/>
-      <c r="C17" s="3"/>
-      <c r="D17" s="3"/>
-      <c r="E17" s="3"/>
-      <c r="F17" s="3"/>
+      <c r="A17" s="1"/>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
     </row>
     <row r="18" spans="1:6" ht="15.6">
-      <c r="A18" s="3"/>
-      <c r="B18" s="13" t="s">
+      <c r="A18" s="1"/>
+      <c r="B18" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C18" s="13"/>
-      <c r="D18" s="3"/>
-      <c r="E18" s="2" t="s">
+      <c r="C18" s="4"/>
+      <c r="D18" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="F18" s="3"/>
+      <c r="E18" s="4"/>
+      <c r="F18" s="4"/>
     </row>
     <row r="19" spans="1:6" ht="15.6">
-      <c r="A19" s="3"/>
-      <c r="B19" s="8" t="s">
+      <c r="A19" s="1"/>
+      <c r="B19" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C19" s="8"/>
-      <c r="D19" s="3"/>
-      <c r="E19" s="1" t="s">
+      <c r="C19" s="5"/>
+      <c r="D19" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="F19" s="3"/>
+      <c r="E19" s="5"/>
+      <c r="F19" s="5"/>
     </row>
   </sheetData>
-  <mergeCells count="13">
+  <mergeCells count="15">
+    <mergeCell ref="C1:F1"/>
+    <mergeCell ref="C2:F3"/>
+    <mergeCell ref="C4:F4"/>
+    <mergeCell ref="A8:F9"/>
+    <mergeCell ref="A10:B11"/>
+    <mergeCell ref="A1:B5"/>
     <mergeCell ref="D16:F16"/>
     <mergeCell ref="B18:C18"/>
     <mergeCell ref="B19:C19"/>
@@ -791,12 +791,8 @@
     <mergeCell ref="D10:F11"/>
     <mergeCell ref="D12:F12"/>
     <mergeCell ref="A12:B12"/>
-    <mergeCell ref="C1:F1"/>
-    <mergeCell ref="C2:F3"/>
-    <mergeCell ref="C4:F4"/>
-    <mergeCell ref="A8:F9"/>
-    <mergeCell ref="A10:B11"/>
-    <mergeCell ref="A1:B5"/>
+    <mergeCell ref="D18:F18"/>
+    <mergeCell ref="D19:F19"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.7" right="0" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>